<commit_message>
P2 - MetalSlug, Fixed avatar width for camera and no shooting while crawling
</commit_message>
<xml_diff>
--- a/Programming2/Game Project/Roca_Alejandro_MetalSlug/MetalSlug/MetalSlug/Resources/Roca_AlejandroMetalSlug.xlsx
+++ b/Programming2/Game Project/Roca_Alejandro_MetalSlug/MetalSlug/MetalSlug/Resources/Roca_AlejandroMetalSlug.xlsx
@@ -42,25 +42,45 @@
     <t xml:space="preserve">Camera</t>
   </si>
   <si>
-    <t xml:space="preserve"> Automatic follow, never leaves boundaries and free moving area</t>
+    <t xml:space="preserve"> - Camera automatically follows the main character.
+ - It never leaves the level boundaries.
+ - It doesn’t move in certain parts like helicopter fights or when it 
+  reaches the end of the level. In these cases, the avatar can move
+   freely without moving the camera.</t>
   </si>
   <si>
     <t xml:space="preserve">Animations</t>
   </si>
   <si>
-    <t xml:space="preserve">Animations for player, enemies, level, projectiles. Death animations…</t>
+    <t xml:space="preserve"> - Main character have animations for shooting, moving, jumping
+   , crawling, pointing up and death animation.
+- All game objects have animations.
+- Some animations are triggered by other game objects like bullet 
+Hitting an enemy and killing which it starts a death animation.
+- Level also have animations for the water and waterfall.
+</t>
   </si>
   <si>
     <t xml:space="preserve">Interactions</t>
   </si>
   <si>
-    <t xml:space="preserve">Killing enemies with projectiles, enemies killing player, item pick up …</t>
+    <t xml:space="preserve"> - Player can release prisoners by hitting them with the avatar shape
+ or shooting a bullet.
+- Enemies are destroyed by using projectiles. Bombs and grenades
+ From the enemies can also kill the player.
+- Player can pick up items by passing through them.</t>
   </si>
   <si>
     <t xml:space="preserve">Game implementation</t>
   </si>
   <si>
-    <t xml:space="preserve">2 types of enemy, prisoner, items, avatar shooting, jumping and crawling..</t>
+    <t xml:space="preserve"> - 2 Different types of enemies with different AI.
+- Prisoners that can be released by 2 different ways (shooting or 
+Passing through). This will end in dropping an Item for the player
+Which can be picked up. 
+- GameObjects are only activated when we are close to them.
+- Different stages where some gameObjects are activated and the 
+Camera doesn’t move until some action happens (kill helicopter)</t>
   </si>
   <si>
     <t xml:space="preserve">HUD and UI</t>
@@ -245,7 +265,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,6 +288,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -359,14 +383,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="91.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -380,47 +404,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -449,7 +473,7 @@
     </row>
     <row r="9" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -474,13 +498,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="A12" activeCellId="1" sqref="C2 A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74"/>
   </cols>
   <sheetData>

</xml_diff>